<commit_message>
Updating excel output file
</commit_message>
<xml_diff>
--- a/output/03522014000163.xlsx
+++ b/output/03522014000163.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bico" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tanque" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Bico" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Tanque" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,7 +460,12 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Obs</t>
+          <t>Obs_relatorio</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Obs_sped</t>
         </is>
       </c>
     </row>
@@ -497,9 +502,10 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -534,9 +540,10 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -571,9 +578,10 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -608,9 +616,10 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -645,9 +654,10 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -682,9 +692,10 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -719,9 +730,10 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -756,9 +768,10 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -793,9 +806,10 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -830,9 +844,10 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -867,9 +882,10 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -904,9 +920,10 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -919,7 +936,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -955,7 +972,12 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Obs</t>
+          <t>Obs_relatorio</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Obs_sped</t>
         </is>
       </c>
     </row>
@@ -987,9 +1009,10 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -1019,9 +1042,10 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1051,9 +1075,10 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1083,9 +1108,10 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1115,9 +1141,10 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1147,9 +1174,10 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1179,9 +1207,10 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>VERDADEIRO</t>
-        </is>
-      </c>
+          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Excel template bug fix
</commit_message>
<xml_diff>
--- a/output/03522014000163.xlsx
+++ b/output/03522014000163.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Bico" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Tanque" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bico" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tanque" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1009,7 +1009,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+          <t>Divergência entre o SPED(954,00) e o relatório(40790,95)!</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
@@ -1042,7 +1042,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+          <t>Divergência entre o SPED(954,00) e o relatório(206100,72)!</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Validado com sucesso! Nenhuma divergência entre o SPED e o relatório foi encontrada!</t>
+          <t>Divergência entre o SPED(954,00) e o relatório(68167,68)!</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>

</xml_diff>